<commit_message>
two screens added misc.
</commit_message>
<xml_diff>
--- a/config/layout/screen1Elements.xlsx
+++ b/config/layout/screen1Elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Python\FinanceManager\config\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBC2922-4DA9-4BC8-A710-C71B78026E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23256DD9-0E3D-497D-A5BC-46A4BB407903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -52,12 +52,6 @@
     <t>textBoxType</t>
   </si>
   <si>
-    <t>lbWelcomeuser</t>
-  </si>
-  <si>
-    <t>Welcome Guest</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -95,6 +89,78 @@
   </si>
   <si>
     <t>placement</t>
+  </si>
+  <si>
+    <t>Financial Summary</t>
+  </si>
+  <si>
+    <t>lbFinancialSummary</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>lbYearSummary</t>
+  </si>
+  <si>
+    <t>lbMonthSummary</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>lbTotalInvestments</t>
+  </si>
+  <si>
+    <t>Total Investments</t>
+  </si>
+  <si>
+    <t>lbTotalCurrentCash</t>
+  </si>
+  <si>
+    <t>Total Cash</t>
+  </si>
+  <si>
+    <t>lbTotalLiabilitites</t>
+  </si>
+  <si>
+    <t>Total Liabilities</t>
+  </si>
+  <si>
+    <t>lbChangeInvestments</t>
+  </si>
+  <si>
+    <t>Net Capital Gains</t>
+  </si>
+  <si>
+    <t>lbChangeCash</t>
+  </si>
+  <si>
+    <t>Net Change in Cash</t>
+  </si>
+  <si>
+    <t>lbChangeLiabilities</t>
+  </si>
+  <si>
+    <t>Net Repayments</t>
+  </si>
+  <si>
+    <t>lbNetGain</t>
+  </si>
+  <si>
+    <t>Net Gain</t>
+  </si>
+  <si>
+    <t>lbTotalWealth</t>
+  </si>
+  <si>
+    <t>Net Current Wealth</t>
+  </si>
+  <si>
+    <t>btAddMonth</t>
+  </si>
+  <si>
+    <t>Add Month</t>
   </si>
 </sst>
 </file>
@@ -456,21 +522,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,17 +547,57 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="E2" s="2"/>
+    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2">
+        <v>100</v>
+      </c>
+      <c r="C2" s="2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -499,13 +606,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150871EB-4912-4180-B17C-83A3764DC5B5}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -518,19 +628,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
@@ -541,7 +651,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2">
         <v>600</v>
@@ -556,28 +666,309 @@
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
       <c r="H3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1">
+        <v>100</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1">
+        <v>100</v>
+      </c>
+      <c r="C6" s="1">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1">
+        <v>100</v>
+      </c>
+      <c r="C8" s="1">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1">
+        <v>100</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1">
+        <v>12</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1">
+        <v>100</v>
+      </c>
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1">
+        <v>100</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1">
+        <v>100</v>
+      </c>
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1">
+        <v>18</v>
+      </c>
+      <c r="I12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -639,49 +1030,49 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Array Struct & Restructure Changes
</commit_message>
<xml_diff>
--- a/config/layout/screen1Elements.xlsx
+++ b/config/layout/screen1Elements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Python\FinanceManager\config\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A99F219-7B3F-4870-ACC5-D8D3AB5A3304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874D5679-591A-42FF-BFB5-3890E23EDCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16080" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>elementSpacing</t>
   </si>
 </sst>
 </file>
@@ -243,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -252,6 +255,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -565,16 +571,16 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="14.1796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +615,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -653,16 +659,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150871EB-4912-4180-B17C-83A3764DC5B5}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +703,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -732,7 +738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -767,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -802,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -837,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -872,7 +878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -907,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -942,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -977,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1012,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1096,13 +1102,13 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1144,7 +1150,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1167,9 +1173,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1177,7 +1183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1191,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +1207,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1209,7 +1215,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1226,13 +1232,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492AD95E-0C52-495E-B79E-5E9671106274}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1254,11 +1260,13 @@
       <c r="G1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1280,10 +1288,12 @@
       <c r="G2">
         <v>80</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1305,10 +1315,12 @@
       <c r="G3">
         <v>-1</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1330,9 +1342,11 @@
       <c r="G4">
         <v>-1</v>
       </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H4" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1353,6 +1367,9 @@
       </c>
       <c r="G5">
         <v>50</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>